<commit_message>
fixing :: in biochemical model examples
</commit_message>
<xml_diff>
--- a/examples/biochemical_model/data.xlsx
+++ b/examples/biochemical_model/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="5850"/>
+    <workbookView windowWidth="21990" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="!!Compound" sheetId="3" r:id="rId1"/>
@@ -266,7 +266,7 @@
     <t>D-Fructose 6-phosphate</t>
   </si>
   <si>
-    <t>kegg.compound::C00085</t>
+    <t>kegg.compound:C00085</t>
   </si>
   <si>
     <t>D_Glucose</t>
@@ -275,7 +275,7 @@
     <t>D-Glucose</t>
   </si>
   <si>
-    <t>kegg.compound::C00031</t>
+    <t>kegg.compound:C00031</t>
   </si>
   <si>
     <t>D_Glucose_6_phosphate</t>
@@ -284,19 +284,19 @@
     <t>D-Glucose 6-phosphate</t>
   </si>
   <si>
-    <t>kegg.compound::C00092</t>
+    <t>kegg.compound:C00092</t>
   </si>
   <si>
     <t>Phosphoenolpyruvate</t>
   </si>
   <si>
-    <t>kegg.compound::C00074</t>
+    <t>kegg.compound:C00074</t>
   </si>
   <si>
     <t>Pyruvate</t>
   </si>
   <si>
-    <t>kegg.compound::C00022</t>
+    <t>kegg.compound:C00022</t>
   </si>
   <si>
     <t>!!ObjTables type='Data' tableFormat='column' id='Model' name='Model' description='Model' date='2020-03-10 22:56:35' objTablesVersion='0.0.8'</t>
@@ -317,7 +317,7 @@
     <t>PGI_R02740</t>
   </si>
   <si>
-    <t>kegg.reaction::R02740</t>
+    <t>kegg.reaction:R02740</t>
   </si>
   <si>
     <t>-1.0 D_Glucose_6_phosphate; 1.0 D_Fructose_6_phosphate</t>
@@ -329,7 +329,7 @@
     <t>PTS_RPTSsy</t>
   </si>
   <si>
-    <t>kegg.reaction::RPTSsy</t>
+    <t>kegg.reaction:RPTSsy</t>
   </si>
   <si>
     <t>-1.0 D_Glucose; -1.0 Phosphoenolpyruvate; 1.0 Pyruvate; 1.0 D_Glucose_6_phosphate</t>
@@ -344,11 +344,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +370,21 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -379,14 +394,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -394,7 +462,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -408,112 +506,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -547,19 +540,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,49 +690,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -625,109 +720,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -741,16 +734,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -760,7 +753,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -769,7 +762,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -789,21 +782,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -815,6 +793,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -841,148 +834,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1346,7 +1339,7 @@
   <sheetPr/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
@@ -1475,11 +1468,11 @@
     <extLst/>
   </autoFilter>
   <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="IsConstant" error="Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="IsConstant" prompt="Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E7" errorStyle="warning">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Identifiers" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="D3:D7" errorStyle="warning">
       <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="IsConstant" error="Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="IsConstant" prompt="Select &quot;True&quot; or &quot;False&quot;." sqref="E3:E7" errorStyle="warning">
-      <formula1>"True,False"</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="C3:C7" errorStyle="warning">
       <formula1>255</formula1>
@@ -1559,7 +1552,7 @@
   <sheetPr/>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
@@ -1656,6 +1649,9 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Gene" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Gene" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="G3:G4" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="IsReversible" error="Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="IsReversible" prompt="Select &quot;True&quot; or &quot;False&quot;." sqref="F3:F4" errorStyle="warning">
+      <formula1>"True,False"</formula1>
+    </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Identifiers" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Identifiers" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="D3:D4" errorStyle="warning">
       <formula1>255</formula1>
     </dataValidation>
@@ -1665,9 +1661,6 @@
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Equation" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Equation" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="E3:E4" errorStyle="warning">
       <formula1>255</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="IsReversible" error="Value must be &quot;True&quot; or &quot;False&quot;." promptTitle="IsReversible" prompt="Select &quot;True&quot; or &quot;False&quot;." sqref="F3:F4" errorStyle="warning">
-      <formula1>"True,False"</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Name" error="Name&#10;&#10;Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Name" prompt="Name&#10;&#10;Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="C3:C4" errorStyle="warning">
       <formula1>255</formula1>

</xml_diff>